<commit_message>
fix microbial fastq orderform
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/microbial_sequencing.1.xlsx
+++ b/tests/fixtures/orderforms/microbial_sequencing.1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincent.janvid/dev/cg/tests/fixtures/orderforms/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsdiazboada/Documents/Clinical_Genomics/repos/cg/tests/fixtures/orderforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F324A78-8DB6-2A40-A270-874ED1AFBE42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F785118-3C9B-2D4C-A38A-B79E764D2613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34180" yWindow="-7060" windowWidth="34520" windowHeight="22840" tabRatio="593" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34220" yWindow="-12800" windowWidth="44200" windowHeight="24240" tabRatio="593" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="6" r:id="rId1"/>
@@ -1491,16 +1491,16 @@
     <t>microbial_sequencing:1</t>
   </si>
   <si>
-    <t>microbialsample1</t>
-  </si>
-  <si>
-    <t>microbialsample2</t>
-  </si>
-  <si>
-    <t>microbialsample3</t>
-  </si>
-  <si>
     <t>Spooky</t>
+  </si>
+  <si>
+    <t>microbialfastqsample1</t>
+  </si>
+  <si>
+    <t>microbialfastqsample2</t>
+  </si>
+  <si>
+    <t>microbialfastqsample3</t>
   </si>
 </sst>
 </file>
@@ -2585,6 +2585,13 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="19" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="19" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2599,13 +2606,6 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="19" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="297">
@@ -3392,7 +3392,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -3436,7 +3436,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -3732,10 +3732,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:W232"/>
+  <dimension ref="A1:Q232"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -3925,22 +3925,22 @@
       <c r="Q8" s="88"/>
     </row>
     <row r="9" spans="1:17" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.15">
-      <c r="A9" s="98" t="s">
+      <c r="A9" s="101" t="s">
         <v>83</v>
       </c>
-      <c r="B9" s="99"/>
-      <c r="C9" s="99"/>
-      <c r="D9" s="99"/>
-      <c r="E9" s="99"/>
-      <c r="F9" s="99"/>
-      <c r="G9" s="99"/>
-      <c r="H9" s="99"/>
-      <c r="I9" s="100"/>
+      <c r="B9" s="102"/>
+      <c r="C9" s="102"/>
+      <c r="D9" s="102"/>
+      <c r="E9" s="102"/>
+      <c r="F9" s="102"/>
+      <c r="G9" s="102"/>
+      <c r="H9" s="102"/>
+      <c r="I9" s="103"/>
       <c r="J9" s="21"/>
-      <c r="K9" s="101" t="s">
+      <c r="K9" s="104" t="s">
         <v>85</v>
       </c>
-      <c r="L9" s="102"/>
+      <c r="L9" s="105"/>
       <c r="M9" s="57"/>
       <c r="N9" s="57"/>
       <c r="O9" s="5" t="s">
@@ -4103,10 +4103,10 @@
       <c r="Q14" s="12"/>
     </row>
     <row r="15" spans="1:17" s="35" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="103" t="s">
-        <v>386</v>
-      </c>
-      <c r="B15" s="104" t="s">
+      <c r="A15" s="98" t="s">
+        <v>387</v>
+      </c>
+      <c r="B15" s="99" t="s">
         <v>374</v>
       </c>
       <c r="C15" s="91" t="s">
@@ -4138,7 +4138,7 @@
       <c r="M15" s="59"/>
       <c r="N15" s="57"/>
       <c r="O15" s="61" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="P15" s="32"/>
       <c r="Q15" s="13" t="s">
@@ -4146,10 +4146,10 @@
       </c>
     </row>
     <row r="16" spans="1:17" s="35" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="103" t="s">
-        <v>387</v>
-      </c>
-      <c r="B16" s="104" t="s">
+      <c r="A16" s="98" t="s">
+        <v>388</v>
+      </c>
+      <c r="B16" s="99" t="s">
         <v>375</v>
       </c>
       <c r="C16" s="91" t="s">
@@ -4189,10 +4189,10 @@
       </c>
     </row>
     <row r="17" spans="1:17" s="35" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="103" t="s">
-        <v>388</v>
-      </c>
-      <c r="B17" s="105"/>
+      <c r="A17" s="98" t="s">
+        <v>389</v>
+      </c>
+      <c r="B17" s="100"/>
       <c r="C17" s="91" t="s">
         <v>384</v>
       </c>

</xml_diff>